<commit_message>
Se modificó la columna de ~
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix-syntax.xlsx
+++ b/src/main/resources/matrix-syntax.xlsx
@@ -1264,11 +1264,11 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="100" workbookViewId="0">
       <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="12.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="4.75"/>
     <col customWidth="1" min="2" max="2" width="13.880000000000001"/>
@@ -25593,7 +25593,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="65" ht="15">
+    <row r="65" ht="14.25">
       <c r="A65" s="1">
         <v>263</v>
       </c>
@@ -25973,7 +25973,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="66" ht="15">
+    <row r="66" ht="14.25">
       <c r="A66" s="1">
         <v>264</v>
       </c>
@@ -26353,7 +26353,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="67" ht="15">
+    <row r="67" ht="14.25">
       <c r="A67" s="1">
         <v>265</v>
       </c>
@@ -26733,7 +26733,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="68" ht="15">
+    <row r="68" ht="14.25">
       <c r="A68" s="1">
         <v>266</v>
       </c>
@@ -27113,7 +27113,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="69" ht="15">
+    <row r="69" ht="14.25">
       <c r="A69" s="1">
         <v>267</v>
       </c>
@@ -27493,7 +27493,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="70" ht="15">
+    <row r="70" ht="14.25">
       <c r="A70" s="1">
         <v>268</v>
       </c>
@@ -27873,7 +27873,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="71" ht="15">
+    <row r="71" ht="14.25">
       <c r="A71" s="1">
         <v>269</v>
       </c>
@@ -28253,7 +28253,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="72" ht="15">
+    <row r="72" ht="14.25">
       <c r="A72" s="1">
         <v>270</v>
       </c>
@@ -28633,7 +28633,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="73" ht="15">
+    <row r="73" ht="14.25">
       <c r="A73" s="1">
         <v>271</v>
       </c>
@@ -29013,7 +29013,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="74" ht="15">
+    <row r="74" ht="14.25">
       <c r="A74" s="1">
         <v>272</v>
       </c>
@@ -29393,7 +29393,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="75" ht="15">
+    <row r="75" ht="14.25">
       <c r="A75" s="1">
         <v>273</v>
       </c>
@@ -29773,7 +29773,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="76" ht="15">
+    <row r="76" ht="14.25">
       <c r="A76" s="1">
         <v>274</v>
       </c>
@@ -30153,7 +30153,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="77" ht="15">
+    <row r="77" ht="14.25">
       <c r="A77" s="1">
         <v>275</v>
       </c>
@@ -30533,7 +30533,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="78" ht="15">
+    <row r="78" ht="14.25">
       <c r="A78" s="1">
         <v>276</v>
       </c>
@@ -30913,7 +30913,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="79" ht="15">
+    <row r="79" ht="14.25">
       <c r="A79" s="1">
         <v>277</v>
       </c>
@@ -31293,7 +31293,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="80" ht="15">
+    <row r="80" ht="14.25">
       <c r="A80" s="1">
         <v>278</v>
       </c>
@@ -31673,7 +31673,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="81" ht="15">
+    <row r="81" ht="14.25">
       <c r="A81" s="1">
         <v>279</v>
       </c>
@@ -32053,7 +32053,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="82" ht="15">
+    <row r="82" ht="14.25">
       <c r="A82" s="1">
         <v>280</v>
       </c>
@@ -32433,7 +32433,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="83" ht="15">
+    <row r="83" ht="14.25">
       <c r="A83" s="1">
         <v>281</v>
       </c>
@@ -32813,7 +32813,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="84" ht="15">
+    <row r="84" ht="14.25">
       <c r="A84" s="1">
         <v>282</v>
       </c>
@@ -33193,7 +33193,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="85" ht="15">
+    <row r="85" ht="14.25">
       <c r="A85" s="1">
         <v>283</v>
       </c>
@@ -33573,7 +33573,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="86" ht="15">
+    <row r="86" ht="14.25">
       <c r="A86" s="1">
         <v>284</v>
       </c>
@@ -33953,7 +33953,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="87" ht="15">
+    <row r="87" ht="14.25">
       <c r="A87" s="1">
         <v>285</v>
       </c>
@@ -33979,7 +33979,7 @@
         <v>523</v>
       </c>
       <c r="I87" s="3">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="J87" s="3">
         <v>523</v>
@@ -34333,7 +34333,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="88" ht="15">
+    <row r="88" ht="14.25">
       <c r="A88" s="1">
         <v>286</v>
       </c>
@@ -34713,7 +34713,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="89" ht="15">
+    <row r="89" ht="14.25">
       <c r="A89" s="1">
         <v>287</v>
       </c>
@@ -35093,7 +35093,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="90" ht="15">
+    <row r="90" ht="14.25">
       <c r="A90" s="1">
         <v>288</v>
       </c>
@@ -35473,7 +35473,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="91" ht="15">
+    <row r="91" ht="14.25">
       <c r="A91" s="1">
         <v>289</v>
       </c>
@@ -35853,7 +35853,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="92" ht="15">
+    <row r="92" ht="14.25">
       <c r="A92" s="1">
         <v>290</v>
       </c>
@@ -36233,7 +36233,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="93" ht="15">
+    <row r="93" ht="14.25">
       <c r="A93" s="1">
         <v>291</v>
       </c>
@@ -36613,7 +36613,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="94" ht="15">
+    <row r="94" ht="14.25">
       <c r="A94" s="1">
         <v>292</v>
       </c>

</xml_diff>

<commit_message>
Se agregó la producción 183
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix-syntax.xlsx
+++ b/src/main/resources/matrix-syntax.xlsx
@@ -675,10 +675,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -703,6 +703,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -710,9 +717,25 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -724,15 +747,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,16 +763,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,7 +780,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -808,17 +817,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -833,14 +840,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,7 +861,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,13 +897,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,151 +1029,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,11 +1064,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1112,6 +1127,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1126,79 +1161,41 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1207,101 +1204,104 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1620,10 +1620,10 @@
   <sheetPr/>
   <dimension ref="A1:DW294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DV1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="EB89" sqref="EB89"/>
+      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="12.75"/>
@@ -2923,7 +2923,7 @@
         <v>508</v>
       </c>
       <c r="AV4" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW4" s="3">
         <v>508</v>
@@ -2995,7 +2995,7 @@
         <v>508</v>
       </c>
       <c r="BT4" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU4" s="3">
         <v>508</v>
@@ -3306,7 +3306,7 @@
         <v>506</v>
       </c>
       <c r="AV5" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW5" s="3">
         <v>506</v>
@@ -3689,7 +3689,7 @@
         <v>508</v>
       </c>
       <c r="AV6" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW6" s="3">
         <v>508</v>
@@ -4072,7 +4072,7 @@
         <v>508</v>
       </c>
       <c r="AV7" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW7" s="3">
         <v>508</v>
@@ -4458,7 +4458,7 @@
         <v>508</v>
       </c>
       <c r="AW8" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX8" s="3">
         <v>508</v>
@@ -5257,7 +5257,7 @@
         <v>508</v>
       </c>
       <c r="BH10" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BI10" s="3">
         <v>508</v>
@@ -5607,7 +5607,7 @@
         <v>509</v>
       </c>
       <c r="AW11" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX11" s="3">
         <v>509</v>
@@ -6385,7 +6385,7 @@
         <v>510</v>
       </c>
       <c r="BA13" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB13" s="3">
         <v>510</v>
@@ -6753,7 +6753,7 @@
         <v>511</v>
       </c>
       <c r="AV14" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW14" s="3">
         <v>511</v>
@@ -7139,7 +7139,7 @@
         <v>508</v>
       </c>
       <c r="AW15" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX15" s="3">
         <v>508</v>
@@ -7917,7 +7917,7 @@
         <v>510</v>
       </c>
       <c r="BA17" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB17" s="3">
         <v>510</v>
@@ -8288,7 +8288,7 @@
         <v>508</v>
       </c>
       <c r="AW18" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX18" s="3">
         <v>508</v>
@@ -8671,7 +8671,7 @@
         <v>508</v>
       </c>
       <c r="AW19" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX19" s="3">
         <v>508</v>
@@ -10981,7 +10981,7 @@
         <v>510</v>
       </c>
       <c r="BA25" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB25" s="3">
         <v>510</v>
@@ -11349,7 +11349,7 @@
         <v>511</v>
       </c>
       <c r="AV26" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW26" s="3">
         <v>511</v>
@@ -11735,7 +11735,7 @@
         <v>508</v>
       </c>
       <c r="AW27" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX27" s="3">
         <v>508</v>
@@ -12130,7 +12130,7 @@
         <v>510</v>
       </c>
       <c r="BA28" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB28" s="3">
         <v>510</v>
@@ -13656,7 +13656,7 @@
         <v>523</v>
       </c>
       <c r="AY32" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ32" s="3">
         <v>47</v>
@@ -14039,7 +14039,7 @@
         <v>510</v>
       </c>
       <c r="AY33" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ33" s="3">
         <v>510</v>
@@ -14326,7 +14326,7 @@
         <v>514</v>
       </c>
       <c r="S34" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T34" s="3">
         <v>514</v>
@@ -14413,7 +14413,7 @@
         <v>514</v>
       </c>
       <c r="AV34" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW34" s="3">
         <v>514</v>
@@ -14485,7 +14485,7 @@
         <v>514</v>
       </c>
       <c r="BT34" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU34" s="3">
         <v>514</v>
@@ -15317,10 +15317,10 @@
         <v>509</v>
       </c>
       <c r="CP36" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CQ36" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CR36" s="3">
         <v>509</v>
@@ -15598,7 +15598,7 @@
         <v>510</v>
       </c>
       <c r="BH37" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BI37" s="3">
         <v>510</v>
@@ -15948,7 +15948,7 @@
         <v>510</v>
       </c>
       <c r="AW38" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX38" s="3">
         <v>510</v>
@@ -17232,10 +17232,10 @@
         <v>509</v>
       </c>
       <c r="CP41" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CQ41" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CR41" s="3">
         <v>509</v>
@@ -17513,7 +17513,7 @@
         <v>510</v>
       </c>
       <c r="BH42" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BI42" s="3">
         <v>510</v>
@@ -17863,7 +17863,7 @@
         <v>510</v>
       </c>
       <c r="AW43" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX43" s="3">
         <v>510</v>
@@ -18189,7 +18189,7 @@
         <v>526</v>
       </c>
       <c r="AD44" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE44" s="3">
         <v>526</v>
@@ -19018,7 +19018,7 @@
         <v>523</v>
       </c>
       <c r="AY46" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ46" s="3">
         <v>68</v>
@@ -19401,7 +19401,7 @@
         <v>510</v>
       </c>
       <c r="AY47" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ47" s="3">
         <v>510</v>
@@ -20544,7 +20544,7 @@
         <v>508</v>
       </c>
       <c r="AW50" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX50" s="3">
         <v>508</v>
@@ -21322,7 +21322,7 @@
         <v>510</v>
       </c>
       <c r="BA52" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB52" s="3">
         <v>510</v>
@@ -21690,7 +21690,7 @@
         <v>511</v>
       </c>
       <c r="AV53" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW53" s="3">
         <v>511</v>
@@ -22076,7 +22076,7 @@
         <v>508</v>
       </c>
       <c r="AW54" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX54" s="3">
         <v>508</v>
@@ -23620,7 +23620,7 @@
         <v>510</v>
       </c>
       <c r="BA58" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB58" s="3">
         <v>510</v>
@@ -23901,7 +23901,7 @@
         <v>530</v>
       </c>
       <c r="S59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T59" s="3">
         <v>530</v>
@@ -23988,10 +23988,10 @@
         <v>530</v>
       </c>
       <c r="AV59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX59" s="3">
         <v>530</v>
@@ -24051,7 +24051,7 @@
         <v>530</v>
       </c>
       <c r="BQ59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR59" s="3">
         <v>530</v>
@@ -24060,7 +24060,7 @@
         <v>530</v>
       </c>
       <c r="BT59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU59" s="3">
         <v>530</v>
@@ -24111,7 +24111,7 @@
         <v>530</v>
       </c>
       <c r="CK59" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL59" s="3">
         <v>530</v>
@@ -24239,7 +24239,7 @@
         <v>531</v>
       </c>
       <c r="D60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E60" s="3">
         <v>531</v>
@@ -24248,13 +24248,13 @@
         <v>531</v>
       </c>
       <c r="G60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H60" s="3">
         <v>531</v>
       </c>
       <c r="I60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J60" s="3">
         <v>531</v>
@@ -24284,7 +24284,7 @@
         <v>531</v>
       </c>
       <c r="S60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T60" s="3">
         <v>531</v>
@@ -24359,7 +24359,7 @@
         <v>531</v>
       </c>
       <c r="AR60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS60" s="3">
         <v>531</v>
@@ -24371,7 +24371,7 @@
         <v>531</v>
       </c>
       <c r="AV60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW60" s="3">
         <v>531</v>
@@ -24383,61 +24383,61 @@
         <v>531</v>
       </c>
       <c r="AZ60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BA60" s="3">
         <v>531</v>
       </c>
       <c r="BB60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BC60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BD60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BE60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BF60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BG60" s="3">
         <v>531</v>
       </c>
       <c r="BH60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BI60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BJ60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BK60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BL60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BM60" s="3">
         <v>531</v>
       </c>
       <c r="BN60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BO60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BP60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BQ60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BS60" s="3">
         <v>531</v>
@@ -24467,34 +24467,34 @@
         <v>531</v>
       </c>
       <c r="CB60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CC60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CD60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CE60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CF60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CG60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CH60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CI60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CJ60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CK60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL60" s="3">
         <v>531</v>
@@ -24518,40 +24518,40 @@
         <v>531</v>
       </c>
       <c r="CS60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CT60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CU60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CV60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CW60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CX60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CY60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CZ60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DA60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DB60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DC60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DD60" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DE60" s="3">
         <v>531</v>
@@ -24877,7 +24877,7 @@
         <v>508</v>
       </c>
       <c r="CK61" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL61" s="3">
         <v>508</v>
@@ -25140,7 +25140,7 @@
         <v>532</v>
       </c>
       <c r="AW62" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX62" s="3">
         <v>532</v>
@@ -25643,7 +25643,7 @@
         <v>508</v>
       </c>
       <c r="CK63" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL63" s="3">
         <v>508</v>
@@ -25906,7 +25906,7 @@
         <v>508</v>
       </c>
       <c r="AW64" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX64" s="3">
         <v>508</v>
@@ -26289,7 +26289,7 @@
         <v>508</v>
       </c>
       <c r="AW65" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX65" s="3">
         <v>508</v>
@@ -26965,7 +26965,7 @@
         <v>510</v>
       </c>
       <c r="S67" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T67" s="3">
         <v>510</v>
@@ -27450,7 +27450,7 @@
         <v>510</v>
       </c>
       <c r="BA68" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB68" s="3">
         <v>510</v>
@@ -28291,7 +28291,7 @@
         <v>528</v>
       </c>
       <c r="BZ70" s="3">
-        <v>528</v>
+        <v>182</v>
       </c>
       <c r="CA70" s="3">
         <v>528</v>
@@ -29742,7 +29742,7 @@
         <v>510</v>
       </c>
       <c r="AY74" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ74" s="3">
         <v>510</v>
@@ -30364,7 +30364,7 @@
         <v>199</v>
       </c>
       <c r="C76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D76" s="3">
         <v>538</v>
@@ -30373,7 +30373,7 @@
         <v>538</v>
       </c>
       <c r="F76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G76" s="3">
         <v>538</v>
@@ -30391,43 +30391,43 @@
         <v>139</v>
       </c>
       <c r="L76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N76" s="3">
         <v>538</v>
       </c>
       <c r="O76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P76" s="3">
         <v>538</v>
       </c>
       <c r="Q76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R76" s="3">
         <v>538</v>
       </c>
       <c r="S76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W76" s="3">
         <v>538</v>
       </c>
       <c r="X76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y76" s="3">
         <v>538</v>
@@ -30439,31 +30439,31 @@
         <v>538</v>
       </c>
       <c r="AB76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC76" s="3">
         <v>538</v>
       </c>
       <c r="AD76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF76" s="3">
         <v>538</v>
       </c>
       <c r="AG76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK76" s="3">
         <v>538</v>
@@ -30472,16 +30472,16 @@
         <v>538</v>
       </c>
       <c r="AM76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN76" s="3">
         <v>538</v>
       </c>
       <c r="AO76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ76" s="3">
         <v>538</v>
@@ -30490,31 +30490,31 @@
         <v>538</v>
       </c>
       <c r="AS76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX76" s="3">
         <v>538</v>
       </c>
       <c r="AY76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ76" s="3">
         <v>538</v>
       </c>
       <c r="BA76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB76" s="3">
         <v>538</v>
@@ -30550,7 +30550,7 @@
         <v>538</v>
       </c>
       <c r="BM76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN76" s="3">
         <v>538</v>
@@ -30562,7 +30562,7 @@
         <v>538</v>
       </c>
       <c r="BQ76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR76" s="3">
         <v>538</v>
@@ -30571,7 +30571,7 @@
         <v>538</v>
       </c>
       <c r="BT76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU76" s="3">
         <v>538</v>
@@ -30622,7 +30622,7 @@
         <v>538</v>
       </c>
       <c r="CK76" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL76" s="3">
         <v>538</v>
@@ -31130,7 +31130,7 @@
         <v>201</v>
       </c>
       <c r="C78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D78" s="3">
         <v>539</v>
@@ -31139,7 +31139,7 @@
         <v>539</v>
       </c>
       <c r="F78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G78" s="3">
         <v>539</v>
@@ -31151,10 +31151,10 @@
         <v>539</v>
       </c>
       <c r="J78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L78" s="3">
         <v>143</v>
@@ -31172,28 +31172,28 @@
         <v>539</v>
       </c>
       <c r="Q78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R78" s="3">
         <v>539</v>
       </c>
       <c r="S78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W78" s="3">
         <v>539</v>
       </c>
       <c r="X78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y78" s="3">
         <v>539</v>
@@ -31205,31 +31205,31 @@
         <v>539</v>
       </c>
       <c r="AB78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC78" s="3">
         <v>539</v>
       </c>
       <c r="AD78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF78" s="3">
         <v>539</v>
       </c>
       <c r="AG78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK78" s="3">
         <v>539</v>
@@ -31238,16 +31238,16 @@
         <v>539</v>
       </c>
       <c r="AM78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN78" s="3">
         <v>539</v>
       </c>
       <c r="AO78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ78" s="3">
         <v>539</v>
@@ -31256,31 +31256,31 @@
         <v>539</v>
       </c>
       <c r="AS78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX78" s="3">
         <v>539</v>
       </c>
       <c r="AY78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ78" s="3">
         <v>539</v>
       </c>
       <c r="BA78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB78" s="3">
         <v>539</v>
@@ -31316,7 +31316,7 @@
         <v>539</v>
       </c>
       <c r="BM78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN78" s="3">
         <v>539</v>
@@ -31328,7 +31328,7 @@
         <v>539</v>
       </c>
       <c r="BQ78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR78" s="3">
         <v>539</v>
@@ -31337,7 +31337,7 @@
         <v>539</v>
       </c>
       <c r="BT78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU78" s="3">
         <v>539</v>
@@ -31388,7 +31388,7 @@
         <v>539</v>
       </c>
       <c r="CK78" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL78" s="3">
         <v>539</v>
@@ -31896,7 +31896,7 @@
         <v>203</v>
       </c>
       <c r="C80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D80" s="3">
         <v>540</v>
@@ -31905,7 +31905,7 @@
         <v>540</v>
       </c>
       <c r="F80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G80" s="3">
         <v>540</v>
@@ -31917,49 +31917,49 @@
         <v>540</v>
       </c>
       <c r="J80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N80" s="3">
         <v>540</v>
       </c>
       <c r="O80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P80" s="3">
         <v>540</v>
       </c>
       <c r="Q80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R80" s="3">
         <v>540</v>
       </c>
       <c r="S80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W80" s="3">
         <v>540</v>
       </c>
       <c r="X80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y80" s="3">
         <v>540</v>
@@ -31971,7 +31971,7 @@
         <v>540</v>
       </c>
       <c r="AB80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC80" s="3">
         <v>540</v>
@@ -31980,7 +31980,7 @@
         <v>146</v>
       </c>
       <c r="AE80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF80" s="3">
         <v>540</v>
@@ -31992,10 +31992,10 @@
         <v>151</v>
       </c>
       <c r="AI80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK80" s="3">
         <v>540</v>
@@ -32028,25 +32028,25 @@
         <v>153</v>
       </c>
       <c r="AU80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX80" s="3">
         <v>540</v>
       </c>
       <c r="AY80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ80" s="3">
         <v>540</v>
       </c>
       <c r="BA80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB80" s="3">
         <v>540</v>
@@ -32082,7 +32082,7 @@
         <v>540</v>
       </c>
       <c r="BM80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN80" s="3">
         <v>540</v>
@@ -32094,7 +32094,7 @@
         <v>540</v>
       </c>
       <c r="BQ80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR80" s="3">
         <v>540</v>
@@ -32103,7 +32103,7 @@
         <v>540</v>
       </c>
       <c r="BT80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU80" s="3">
         <v>540</v>
@@ -32154,7 +32154,7 @@
         <v>540</v>
       </c>
       <c r="CK80" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL80" s="3">
         <v>540</v>
@@ -32683,49 +32683,49 @@
         <v>541</v>
       </c>
       <c r="J82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N82" s="3">
         <v>541</v>
       </c>
       <c r="O82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P82" s="3">
         <v>541</v>
       </c>
       <c r="Q82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R82" s="3">
         <v>541</v>
       </c>
       <c r="S82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W82" s="3">
         <v>541</v>
       </c>
       <c r="X82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y82" s="3">
         <v>541</v>
@@ -32737,13 +32737,13 @@
         <v>541</v>
       </c>
       <c r="AB82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC82" s="3">
         <v>541</v>
       </c>
       <c r="AD82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE82" s="3">
         <v>157</v>
@@ -32752,10 +32752,10 @@
         <v>541</v>
       </c>
       <c r="AG82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI82" s="3">
         <v>158</v>
@@ -32770,16 +32770,16 @@
         <v>541</v>
       </c>
       <c r="AM82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN82" s="3">
         <v>541</v>
       </c>
       <c r="AO82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ82" s="3">
         <v>541</v>
@@ -32788,31 +32788,31 @@
         <v>541</v>
       </c>
       <c r="AS82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX82" s="3">
         <v>541</v>
       </c>
       <c r="AY82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ82" s="3">
         <v>541</v>
       </c>
       <c r="BA82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB82" s="3">
         <v>541</v>
@@ -32848,7 +32848,7 @@
         <v>541</v>
       </c>
       <c r="BM82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN82" s="3">
         <v>541</v>
@@ -32860,7 +32860,7 @@
         <v>541</v>
       </c>
       <c r="BQ82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR82" s="3">
         <v>541</v>
@@ -32869,7 +32869,7 @@
         <v>541</v>
       </c>
       <c r="BT82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU82" s="3">
         <v>541</v>
@@ -32920,7 +32920,7 @@
         <v>541</v>
       </c>
       <c r="CK82" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL82" s="3">
         <v>541</v>
@@ -33428,7 +33428,7 @@
         <v>207</v>
       </c>
       <c r="C84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D84" s="3">
         <v>542</v>
@@ -33437,7 +33437,7 @@
         <v>542</v>
       </c>
       <c r="F84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G84" s="3">
         <v>542</v>
@@ -33449,43 +33449,43 @@
         <v>542</v>
       </c>
       <c r="J84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N84" s="3">
         <v>542</v>
       </c>
       <c r="O84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P84" s="3">
         <v>542</v>
       </c>
       <c r="Q84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R84" s="3">
         <v>542</v>
       </c>
       <c r="S84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U84" s="3">
         <v>161</v>
       </c>
       <c r="V84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W84" s="3">
         <v>542</v>
@@ -33509,25 +33509,25 @@
         <v>542</v>
       </c>
       <c r="AD84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF84" s="3">
         <v>542</v>
       </c>
       <c r="AG84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK84" s="3">
         <v>542</v>
@@ -33536,16 +33536,16 @@
         <v>542</v>
       </c>
       <c r="AM84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN84" s="3">
         <v>542</v>
       </c>
       <c r="AO84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ84" s="3">
         <v>542</v>
@@ -33554,31 +33554,31 @@
         <v>542</v>
       </c>
       <c r="AS84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX84" s="3">
         <v>542</v>
       </c>
       <c r="AY84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ84" s="3">
         <v>542</v>
       </c>
       <c r="BA84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB84" s="3">
         <v>542</v>
@@ -33614,7 +33614,7 @@
         <v>542</v>
       </c>
       <c r="BM84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN84" s="3">
         <v>542</v>
@@ -33626,7 +33626,7 @@
         <v>542</v>
       </c>
       <c r="BQ84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR84" s="3">
         <v>542</v>
@@ -33635,7 +33635,7 @@
         <v>542</v>
       </c>
       <c r="BT84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU84" s="3">
         <v>542</v>
@@ -33686,7 +33686,7 @@
         <v>542</v>
       </c>
       <c r="CK84" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL84" s="3">
         <v>542</v>
@@ -34194,7 +34194,7 @@
         <v>209</v>
       </c>
       <c r="C86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D86" s="3">
         <v>543</v>
@@ -34203,7 +34203,7 @@
         <v>543</v>
       </c>
       <c r="F86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G86" s="3">
         <v>543</v>
@@ -34215,40 +34215,40 @@
         <v>543</v>
       </c>
       <c r="J86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N86" s="3">
         <v>543</v>
       </c>
       <c r="O86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P86" s="3">
         <v>543</v>
       </c>
       <c r="Q86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R86" s="3">
         <v>543</v>
       </c>
       <c r="S86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V86" s="3">
         <v>165</v>
@@ -34257,7 +34257,7 @@
         <v>543</v>
       </c>
       <c r="X86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y86" s="3">
         <v>543</v>
@@ -34269,31 +34269,31 @@
         <v>543</v>
       </c>
       <c r="AB86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC86" s="3">
         <v>543</v>
       </c>
       <c r="AD86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF86" s="3">
         <v>543</v>
       </c>
       <c r="AG86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK86" s="3">
         <v>543</v>
@@ -34302,16 +34302,16 @@
         <v>543</v>
       </c>
       <c r="AM86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN86" s="3">
         <v>543</v>
       </c>
       <c r="AO86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ86" s="3">
         <v>543</v>
@@ -34320,31 +34320,31 @@
         <v>543</v>
       </c>
       <c r="AS86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX86" s="3">
         <v>543</v>
       </c>
       <c r="AY86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ86" s="3">
         <v>543</v>
       </c>
       <c r="BA86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB86" s="3">
         <v>543</v>
@@ -34380,7 +34380,7 @@
         <v>543</v>
       </c>
       <c r="BM86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN86" s="3">
         <v>543</v>
@@ -34392,7 +34392,7 @@
         <v>543</v>
       </c>
       <c r="BQ86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR86" s="3">
         <v>543</v>
@@ -34401,7 +34401,7 @@
         <v>543</v>
       </c>
       <c r="BT86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU86" s="3">
         <v>543</v>
@@ -34452,7 +34452,7 @@
         <v>543</v>
       </c>
       <c r="CK86" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL86" s="3">
         <v>543</v>
@@ -35131,7 +35131,7 @@
         <v>545</v>
       </c>
       <c r="BH88" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BI88" s="3">
         <v>545</v>
@@ -35343,7 +35343,7 @@
         <v>212</v>
       </c>
       <c r="C89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3">
         <v>546</v>
@@ -35352,7 +35352,7 @@
         <v>181</v>
       </c>
       <c r="F89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G89" s="3">
         <v>546</v>
@@ -35364,49 +35364,49 @@
         <v>546</v>
       </c>
       <c r="J89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N89" s="3">
         <v>181</v>
       </c>
       <c r="O89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P89" s="3">
         <v>181</v>
       </c>
       <c r="Q89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R89" s="3">
         <v>546</v>
       </c>
       <c r="S89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W89" s="3">
         <v>181</v>
       </c>
       <c r="X89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y89" s="3">
         <v>546</v>
@@ -35418,31 +35418,31 @@
         <v>546</v>
       </c>
       <c r="AB89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC89" s="3">
         <v>181</v>
       </c>
       <c r="AD89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF89" s="3">
         <v>181</v>
       </c>
       <c r="AG89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK89" s="3">
         <v>181</v>
@@ -35451,16 +35451,16 @@
         <v>181</v>
       </c>
       <c r="AM89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN89" s="3">
         <v>181</v>
       </c>
       <c r="AO89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ89" s="3">
         <v>546</v>
@@ -35469,31 +35469,31 @@
         <v>546</v>
       </c>
       <c r="AS89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX89" s="3">
         <v>172</v>
       </c>
       <c r="AY89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ89" s="3">
         <v>173</v>
       </c>
       <c r="BA89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB89" s="3">
         <v>546</v>
@@ -35529,7 +35529,7 @@
         <v>546</v>
       </c>
       <c r="BM89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN89" s="3">
         <v>546</v>
@@ -35541,7 +35541,7 @@
         <v>546</v>
       </c>
       <c r="BQ89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR89" s="3">
         <v>546</v>
@@ -35550,7 +35550,7 @@
         <v>546</v>
       </c>
       <c r="BT89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU89" s="3">
         <v>546</v>
@@ -35601,7 +35601,7 @@
         <v>546</v>
       </c>
       <c r="CK89" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL89" s="3">
         <v>546</v>
@@ -35726,7 +35726,7 @@
         <v>213</v>
       </c>
       <c r="C90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D90" s="3">
         <v>527</v>
@@ -35735,7 +35735,7 @@
         <v>174</v>
       </c>
       <c r="F90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G90" s="3">
         <v>527</v>
@@ -35747,49 +35747,49 @@
         <v>527</v>
       </c>
       <c r="J90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N90" s="3">
         <v>174</v>
       </c>
       <c r="O90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P90" s="3">
         <v>174</v>
       </c>
       <c r="Q90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R90" s="3">
         <v>527</v>
       </c>
       <c r="S90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W90" s="3">
         <v>174</v>
       </c>
       <c r="X90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y90" s="3">
         <v>527</v>
@@ -35801,31 +35801,31 @@
         <v>527</v>
       </c>
       <c r="AB90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC90" s="3">
         <v>174</v>
       </c>
       <c r="AD90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF90" s="3">
         <v>174</v>
       </c>
       <c r="AG90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK90" s="3">
         <v>174</v>
@@ -35834,16 +35834,16 @@
         <v>174</v>
       </c>
       <c r="AM90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN90" s="3">
         <v>174</v>
       </c>
       <c r="AO90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ90" s="3">
         <v>527</v>
@@ -35852,31 +35852,31 @@
         <v>527</v>
       </c>
       <c r="AS90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AV90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX90" s="3">
         <v>527</v>
       </c>
       <c r="AY90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ90" s="3">
         <v>527</v>
       </c>
       <c r="BA90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB90" s="3">
         <v>527</v>
@@ -35912,7 +35912,7 @@
         <v>527</v>
       </c>
       <c r="BM90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN90" s="3">
         <v>527</v>
@@ -35924,7 +35924,7 @@
         <v>527</v>
       </c>
       <c r="BQ90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR90" s="3">
         <v>527</v>
@@ -35933,7 +35933,7 @@
         <v>527</v>
       </c>
       <c r="BT90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU90" s="3">
         <v>527</v>
@@ -35984,7 +35984,7 @@
         <v>527</v>
       </c>
       <c r="CK90" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL90" s="3">
         <v>527</v>
@@ -36109,7 +36109,7 @@
         <v>214</v>
       </c>
       <c r="C91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D91" s="3">
         <v>547</v>
@@ -36118,7 +36118,7 @@
         <v>547</v>
       </c>
       <c r="F91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G91" s="3">
         <v>547</v>
@@ -36130,49 +36130,49 @@
         <v>547</v>
       </c>
       <c r="J91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N91" s="3">
         <v>547</v>
       </c>
       <c r="O91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P91" s="3">
         <v>547</v>
       </c>
       <c r="Q91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R91" s="3">
         <v>547</v>
       </c>
       <c r="S91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W91" s="3">
         <v>547</v>
       </c>
       <c r="X91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y91" s="3">
         <v>547</v>
@@ -36184,31 +36184,31 @@
         <v>547</v>
       </c>
       <c r="AB91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC91" s="3">
         <v>547</v>
       </c>
       <c r="AD91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF91" s="3">
         <v>547</v>
       </c>
       <c r="AG91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AJ91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK91" s="3">
         <v>547</v>
@@ -36217,16 +36217,16 @@
         <v>547</v>
       </c>
       <c r="AM91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN91" s="3">
         <v>547</v>
       </c>
       <c r="AO91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ91" s="3">
         <v>547</v>
@@ -36235,31 +36235,31 @@
         <v>547</v>
       </c>
       <c r="AS91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AU91" s="3">
         <v>175</v>
       </c>
       <c r="AV91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX91" s="3">
         <v>547</v>
       </c>
       <c r="AY91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ91" s="3">
         <v>547</v>
       </c>
       <c r="BA91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB91" s="3">
         <v>547</v>
@@ -36295,7 +36295,7 @@
         <v>547</v>
       </c>
       <c r="BM91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN91" s="3">
         <v>547</v>
@@ -36307,7 +36307,7 @@
         <v>547</v>
       </c>
       <c r="BQ91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR91" s="3">
         <v>547</v>
@@ -36316,7 +36316,7 @@
         <v>547</v>
       </c>
       <c r="BT91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU91" s="3">
         <v>547</v>
@@ -36367,7 +36367,7 @@
         <v>547</v>
       </c>
       <c r="CK91" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL91" s="3">
         <v>547</v>
@@ -36642,7 +36642,7 @@
         <v>176</v>
       </c>
       <c r="BA92" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB92" s="3">
         <v>176</v>
@@ -37025,7 +37025,7 @@
         <v>510</v>
       </c>
       <c r="BA93" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB93" s="3">
         <v>510</v>
@@ -37405,7 +37405,7 @@
         <v>548</v>
       </c>
       <c r="AZ94" s="3">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BA94" s="3">
         <v>548</v>
@@ -59831,7 +59831,7 @@
   </sheetData>
   <conditionalFormatting sqref="C2:DW94">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>182</formula>
+      <formula>183</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>499</formula>

</xml_diff>

<commit_message>
Se arregló el problema con el tipo #
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix-syntax.xlsx
+++ b/src/main/resources/matrix-syntax.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7755" tabRatio="322"/>
+    <workbookView windowWidth="20490" windowHeight="8835" tabRatio="322"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -673,12 +673,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -703,55 +703,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -763,34 +717,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -817,8 +748,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -831,16 +810,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,7 +861,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,7 +909,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -885,31 +951,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,67 +963,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -993,25 +975,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,7 +993,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,16 +1065,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,6 +1098,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1108,41 +1123,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1161,147 +1141,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1311,59 +1311,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
     <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Salida" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="19" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Énfasis1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Énfasis1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Énfasis1" xfId="28" builtinId="32"/>
+    <cellStyle name="Énfasis2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="40" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Énfasis5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Énfasis5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Énfasis5" xfId="44" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Énfasis6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1620,10 +1620,10 @@
   <sheetPr/>
   <dimension ref="A1:DW294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <selection pane="bottomLeft" activeCell="BG30" sqref="BG30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="12.75"/>
@@ -12531,7 +12531,7 @@
         <v>520</v>
       </c>
       <c r="BG29" s="3">
-        <v>520</v>
+        <v>50</v>
       </c>
       <c r="BH29" s="3">
         <v>57</v>
@@ -12914,7 +12914,7 @@
         <v>521</v>
       </c>
       <c r="BG30" s="3">
-        <v>521</v>
+        <v>44</v>
       </c>
       <c r="BH30" s="3">
         <v>45</v>

</xml_diff>